<commit_message>
Planning in de proftaak rapportage ge-update en speelstukken render functies toegevoegd
</commit_message>
<xml_diff>
--- a/Documentatie - Subdeliverables/Feedback Sheet.xlsx
+++ b/Documentatie - Subdeliverables/Feedback Sheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C513EB-A65D-4796-915B-248C52708AC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEA698B-C7F5-48B0-B090-A3054E1AC294}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -884,7 +884,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>